<commit_message>
bugs fixed and re run
</commit_message>
<xml_diff>
--- a/flow_recs/flow_recs_willow_workings.xlsx
+++ b/flow_recs/flow_recs_willow_workings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieirving/Documents/git/flow_eco_mech/flow_recs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28724D2C-87B6-124A-BEE4-367DCDD4FABD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043EBEFE-D44A-BA43-B4CC-1983722FA2E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="1860" windowWidth="26840" windowHeight="15940" xr2:uid="{424AD499-A585-D54A-A072-11066C252891}"/>
+    <workbookView xWindow="3260" yWindow="1720" windowWidth="15620" windowHeight="15940" activeTab="1" xr2:uid="{424AD499-A585-D54A-A072-11066C252891}"/>
   </bookViews>
   <sheets>
     <sheet name="Willow" sheetId="1" r:id="rId1"/>
+    <sheet name="Typha" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
   <si>
     <t>Willow growth</t>
   </si>
@@ -301,13 +302,100 @@
   </si>
   <si>
     <t>concrete</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Typha growth</t>
+  </si>
+  <si>
+    <t>Typha adult</t>
+  </si>
+  <si>
+    <t>&lt;23 &amp; &gt;71</t>
+  </si>
+  <si>
+    <t>6-1419</t>
+  </si>
+  <si>
+    <t>135-994</t>
+  </si>
+  <si>
+    <t>0.45-52</t>
+  </si>
+  <si>
+    <t>0.45-0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try an over bank </t>
+  </si>
+  <si>
+    <t>23-196</t>
+  </si>
+  <si>
+    <t>83-1968</t>
+  </si>
+  <si>
+    <t>293-1418</t>
+  </si>
+  <si>
+    <t>23-28</t>
+  </si>
+  <si>
+    <t>23-10</t>
+  </si>
+  <si>
+    <t>could try ROB but it is the main channel</t>
+  </si>
+  <si>
+    <t>values are correct, cannot achieve high vewlocity - model resolution issue</t>
+  </si>
+  <si>
+    <t>does not reach high limit</t>
+  </si>
+  <si>
+    <t>23-568</t>
+  </si>
+  <si>
+    <t>23-165</t>
+  </si>
+  <si>
+    <t>77-1703</t>
+  </si>
+  <si>
+    <t>270-1237</t>
+  </si>
+  <si>
+    <t>24-48</t>
+  </si>
+  <si>
+    <t>24-1242</t>
+  </si>
+  <si>
+    <t>93-823</t>
+  </si>
+  <si>
+    <t>23-65</t>
+  </si>
+  <si>
+    <t>52-113</t>
+  </si>
+  <si>
+    <t>26-1486</t>
+  </si>
+  <si>
+    <t>26-586</t>
+  </si>
+  <si>
+    <t>91-1010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +441,18 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -390,6 +490,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C44ECAE-18BD-9B44-A259-6876D2537660}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,4 +1526,926 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08258E46-6C5B-3845-AB5F-F130D4BBDC74}">
+  <dimension ref="A1:I91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>0.45473939180374101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>7.6612300872802699</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="E8" s="6"/>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13">
+        <v>22.984325408935501</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="E14" s="6"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>24.5054531097412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25">
+        <v>26.229257579999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>11101250</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48">
+        <v>0.45473939180374101</v>
+      </c>
+      <c r="H48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53">
+        <v>23.112771987915</v>
+      </c>
+      <c r="H53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E59" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59">
+        <v>22.98432541</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" t="s">
+        <v>112</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65">
+        <v>24.5054531097412</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71">
+        <v>26.229257579999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D72" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>11101250</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figures for flow recs, min limit revised
</commit_message>
<xml_diff>
--- a/flow_recs/flow_recs_willow_workings.xlsx
+++ b/flow_recs/flow_recs_willow_workings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieirving/Documents/git/flow_eco_mech/flow_recs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2E284-1B15-994C-A06E-3D1F39C23A87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C41CCD5-FD51-CB43-8CEC-2D79784AEDA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="1080" windowWidth="25480" windowHeight="15940" activeTab="4" xr2:uid="{424AD499-A585-D54A-A072-11066C252891}"/>
+    <workbookView xWindow="3840" yWindow="1820" windowWidth="25480" windowHeight="15940" xr2:uid="{424AD499-A585-D54A-A072-11066C252891}"/>
   </bookViews>
   <sheets>
     <sheet name="Willow" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="224">
   <si>
     <t>LA202</t>
   </si>
@@ -541,24 +541,6 @@
     <t>30-60</t>
   </si>
   <si>
-    <t>998-5462</t>
-  </si>
-  <si>
-    <t>1945-4763</t>
-  </si>
-  <si>
-    <t>35-707</t>
-  </si>
-  <si>
-    <t>85-506</t>
-  </si>
-  <si>
-    <t>794-4370</t>
-  </si>
-  <si>
-    <t>999-3781</t>
-  </si>
-  <si>
     <t>18-430</t>
   </si>
   <si>
@@ -653,13 +635,88 @@
   </si>
   <si>
     <t>&gt;336</t>
+  </si>
+  <si>
+    <t>44-615</t>
+  </si>
+  <si>
+    <t>136-482</t>
+  </si>
+  <si>
+    <t>13-870</t>
+  </si>
+  <si>
+    <t>24-415</t>
+  </si>
+  <si>
+    <t>64-326</t>
+  </si>
+  <si>
+    <t>7.66-1597</t>
+  </si>
+  <si>
+    <t>7911-9004</t>
+  </si>
+  <si>
+    <t>7911-8558</t>
+  </si>
+  <si>
+    <t>&gt;1278</t>
+  </si>
+  <si>
+    <t>1278-1646</t>
+  </si>
+  <si>
+    <t>1278-1502</t>
+  </si>
+  <si>
+    <t>424-841</t>
+  </si>
+  <si>
+    <t>424-655</t>
+  </si>
+  <si>
+    <t>23-250</t>
+  </si>
+  <si>
+    <t>23-149</t>
+  </si>
+  <si>
+    <t>446-844</t>
+  </si>
+  <si>
+    <t>446-666</t>
+  </si>
+  <si>
+    <t>26-159</t>
+  </si>
+  <si>
+    <t>26-39</t>
+  </si>
+  <si>
+    <t>54-114</t>
+  </si>
+  <si>
+    <t>54-86</t>
+  </si>
+  <si>
+    <t>285-301</t>
+  </si>
+  <si>
+    <t>285-298</t>
+  </si>
+  <si>
+    <t>36-487</t>
+  </si>
+  <si>
+    <t>36-269</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -725,6 +782,13 @@
       <sz val="11"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -746,12 +810,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,6 +830,13 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C44ECAE-18BD-9B44-A259-6876D2537660}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,11 +1224,11 @@
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="I3" t="s">
@@ -1172,21 +1240,25 @@
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1195,11 +1267,11 @@
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>162</v>
       </c>
       <c r="G6" t="s">
@@ -1220,11 +1292,11 @@
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>160</v>
       </c>
       <c r="I7" t="s">
@@ -1236,7 +1308,15 @@
       <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1288,7 +1368,7 @@
       <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I12" t="s">
@@ -1300,26 +1380,32 @@
       <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D13" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" t="s">
+        <v>211</v>
+      </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1349,7 +1435,7 @@
       <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>42</v>
       </c>
       <c r="I18" t="s">
@@ -1361,7 +1447,13 @@
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="D19" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I19" t="s">
@@ -1369,21 +1461,21 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -1416,7 +1508,7 @@
       <c r="D24" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1425,48 +1517,54 @@
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="D25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="8"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -1499,7 +1597,7 @@
       <c r="D30" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>63</v>
       </c>
       <c r="I30" t="s">
@@ -1511,7 +1609,13 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="D31" t="s">
+        <v>216</v>
+      </c>
+      <c r="E31" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I31" t="s">
@@ -1519,21 +1623,21 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -1566,7 +1670,7 @@
       <c r="D35" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1575,22 +1679,28 @@
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="D36" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>72</v>
       </c>
       <c r="I36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -1619,11 +1729,11 @@
       <c r="B40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>62</v>
       </c>
       <c r="I40" t="s">
@@ -1637,25 +1747,31 @@
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="D41" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>58</v>
       </c>
       <c r="I41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
+    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -1684,11 +1800,11 @@
       <c r="B46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6" t="s">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1696,22 +1812,28 @@
       <c r="B47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="D47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1820,44 +1942,44 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1929,16 +2051,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="1"/>
@@ -1991,7 +2113,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5"/>
       <c r="H8" t="s">
         <v>109</v>
       </c>
@@ -2003,35 +2125,35 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2058,7 +2180,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="5"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2067,33 +2189,33 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -2118,40 +2240,40 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -2176,27 +2298,27 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="E26" s="6"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="8"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -2209,31 +2331,31 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -2245,43 +2367,43 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -2293,34 +2415,34 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2365,15 +2487,15 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11" t="s">
+    <row r="49" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="11" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2432,7 +2554,7 @@
       <c r="D54" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="11" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2441,33 +2563,33 @@
       <c r="B55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B56" s="1"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -2497,7 +2619,7 @@
       <c r="D60" t="s">
         <v>110</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="11" t="s">
         <v>63</v>
       </c>
       <c r="H60" t="s">
@@ -2509,33 +2631,33 @@
       <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
@@ -2565,7 +2687,7 @@
       <c r="D66" t="s">
         <v>117</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2574,33 +2696,33 @@
       <c r="B67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="8"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="5"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
@@ -2630,7 +2752,7 @@
       <c r="D72" t="s">
         <v>120</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2639,20 +2761,20 @@
       <c r="B73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B74" s="1"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="8"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="8"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2667,31 +2789,31 @@
       <c r="B77" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E77" s="10"/>
+      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
@@ -2705,43 +2827,43 @@
       <c r="B82" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" s="1"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="5"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
@@ -2755,34 +2877,34 @@
       <c r="B88" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B89" s="1"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2794,13 +2916,13 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H39"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="12"/>
+    <col min="4" max="6" width="10.83203125" style="11"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2811,13 +2933,13 @@
       <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
@@ -2834,10 +2956,10 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>134</v>
       </c>
       <c r="G2" t="s">
@@ -2852,11 +2974,11 @@
       <c r="B3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2865,7 +2987,7 @@
       <c r="B4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2875,18 +2997,18 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2896,10 +3018,10 @@
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>141</v>
       </c>
       <c r="G7" t="s">
@@ -2914,10 +3036,10 @@
       <c r="B8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2926,7 +3048,7 @@
       <c r="B9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -2934,31 +3056,31 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="K10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="K11" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="K12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2970,10 +3092,10 @@
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>144</v>
       </c>
       <c r="G13" t="s">
@@ -2991,10 +3113,10 @@
       <c r="B14" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>146</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -3006,7 +3128,7 @@
       <c r="B15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>147</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -3014,31 +3136,31 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
       <c r="K16" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="K17" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="K18" s="1" t="s">
         <v>130</v>
       </c>
@@ -3050,10 +3172,10 @@
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>149</v>
       </c>
       <c r="G19" t="s">
@@ -3071,10 +3193,10 @@
       <c r="B20" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>151</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3086,7 +3208,7 @@
       <c r="B21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>45</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -3094,26 +3216,26 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="E22" s="14"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -3122,10 +3244,10 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>153</v>
       </c>
       <c r="G25" t="s">
@@ -3140,10 +3262,10 @@
       <c r="B26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3157,19 +3279,19 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="E28" s="14"/>
+      <c r="C28" s="3"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="C29" s="3"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -3187,7 +3309,7 @@
       <c r="B31" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -3196,18 +3318,18 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -3224,7 +3346,7 @@
       <c r="B36" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
@@ -3232,26 +3354,26 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -3268,7 +3390,7 @@
       <c r="B42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
@@ -3276,20 +3398,20 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3300,8 +3422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98868F43-95AF-034B-9F5A-924E43B3E2AC}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H57"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3316,13 +3438,13 @@
       <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
@@ -3336,9 +3458,9 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
@@ -3353,87 +3475,93 @@
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="K6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="3"/>
       <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="3"/>
       <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="F9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <v>7.66</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3443,13 +3571,13 @@
       <c r="B10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F10" s="12"/>
+      <c r="D10" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="11"/>
       <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3457,39 +3585,39 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -3498,63 +3626,69 @@
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="F15" s="12"/>
+      <c r="D15" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="15">
+        <v>22.984325399999999</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -3563,43 +3697,43 @@
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="12"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -3608,47 +3742,47 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -3657,83 +3791,83 @@
       <c r="B31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F31" s="12"/>
+      <c r="D31" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
       <c r="K34" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="3"/>
       <c r="K35" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="4"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="3"/>
       <c r="K36" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="F37" s="12"/>
+      <c r="D37" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" s="11"/>
       <c r="K37" s="1" t="s">
         <v>7</v>
       </c>
@@ -3743,9 +3877,9 @@
       <c r="B38" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
       <c r="K38" s="1" t="s">
         <v>8</v>
       </c>
@@ -3753,39 +3887,39 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="4"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -3794,59 +3928,65 @@
       <c r="B43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="12"/>
+      <c r="D43" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="15">
+        <v>22.984325399999999</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="12"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="4"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -3855,43 +3995,43 @@
       <c r="B49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B52" s="1"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="12"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
+      <c r="A53" s="4"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
@@ -3900,36 +4040,36 @@
       <c r="B54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="12"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="11"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3940,7 +4080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C0F6AF-BA62-5A49-9975-A49839EAE4BB}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3952,12 +4092,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
@@ -3971,7 +4111,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="13"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3979,13 +4119,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>185</v>
+      <c r="D3" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -3997,87 +4137,87 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>186</v>
+      <c r="D4" s="11" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>191</v>
+      <c r="D5" s="11" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>187</v>
+      <c r="D6" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>188</v>
+      <c r="D7" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>189</v>
+      <c r="D11" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -4092,28 +4232,28 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>192</v>
+      <c r="D12" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>190</v>
+      <c r="D13" s="11" t="s">
+        <v>184</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>5</v>
@@ -4122,58 +4262,58 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>193</v>
+      <c r="D14" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>194</v>
+      <c r="D15" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="11"/>
       <c r="I16" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="3"/>
       <c r="I17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="3"/>
       <c r="I18" s="1" t="s">
         <v>7</v>
       </c>
@@ -4183,13 +4323,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>195</v>
+      <c r="D19" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>26</v>
@@ -4204,13 +4344,13 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>198</v>
+      <c r="D20" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>127</v>
@@ -4219,13 +4359,13 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>196</v>
+      <c r="D21" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>128</v>
@@ -4234,58 +4374,58 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>199</v>
+      <c r="D22" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>197</v>
+      <c r="D23" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="11"/>
       <c r="I24" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="3"/>
       <c r="I25" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="3"/>
       <c r="I26" s="1" t="s">
         <v>91</v>
       </c>
@@ -4295,13 +4435,13 @@
         <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>200</v>
+      <c r="D27" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>19</v>
@@ -4316,76 +4456,76 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>202</v>
+      <c r="D28" s="11" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>201</v>
+      <c r="D29" s="11" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>203</v>
+      <c r="D30" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>204</v>
+      <c r="D31" s="11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="12"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="14"/>
+      <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="1" t="s">
         <v>18</v>
       </c>
@@ -4396,227 +4536,227 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="4"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="12"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="4"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="4"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="12"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="12"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="12"/>
+      <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="12"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="4"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="4"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="12"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="12"/>
+      <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="12"/>
+      <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="4"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="4"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="12"/>
+      <c r="D59" s="11"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="11"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="12"/>
+      <c r="D61" s="11"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="12"/>
+      <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="14"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="12"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="12"/>
+      <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="12"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="4"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>